<commit_message>
Added create / delete logic
</commit_message>
<xml_diff>
--- a/api/config/ApiParameters.xlsx
+++ b/api/config/ApiParameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neil\source\repos\ka-member\api\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F921B73-DCB0-4F43-97B4-C957576E47EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A203F94-3C92-4CD1-9253-30091943A874}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="2790" windowWidth="17070" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -717,7 +717,7 @@
   <dimension ref="A1:V75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,81 +1985,81 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
-        <f>C1&amp;" = :"&amp;C1&amp;","</f>
+        <f t="shared" ref="B41:B51" si="40">C1&amp;" = :"&amp;C1&amp;","</f>
         <v>id = :id,</v>
       </c>
       <c r="D41" t="str">
-        <f>""""&amp;C1&amp;""" =&gt; $member-&gt;"&amp;C1&amp;","</f>
+        <f t="shared" ref="D41:D51" si="41">""""&amp;C1&amp;""" =&gt; $member-&gt;"&amp;C1&amp;","</f>
         <v>"id" =&gt; $member-&gt;id,</v>
       </c>
       <c r="H41" t="str">
-        <f>"$this-&gt;"&amp;C1&amp;" = $row['"&amp;C1&amp;"'];"</f>
+        <f t="shared" ref="H41:H51" si="42">"$this-&gt;"&amp;C1&amp;" = $row['"&amp;C1&amp;"'];"</f>
         <v>$this-&gt;id = $row['id'];</v>
       </c>
       <c r="L41" t="str">
-        <f>"$member-&gt;"&amp;C1&amp;" = $data-&gt;"&amp;C1&amp;";"</f>
-        <v>$member-&gt;id = $data-&gt;id;</v>
+        <f>"$item-&gt;"&amp;C1&amp;" = $data-&gt;"&amp;C1&amp;";"</f>
+        <v>$item-&gt;id = $data-&gt;id;</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
-        <f>C2&amp;" = :"&amp;C2&amp;","</f>
+        <f t="shared" si="40"/>
         <v>title = :title,</v>
       </c>
       <c r="D42" t="str">
-        <f>""""&amp;C2&amp;""" =&gt; $member-&gt;"&amp;C2&amp;","</f>
+        <f t="shared" si="41"/>
         <v>"title" =&gt; $member-&gt;title,</v>
       </c>
       <c r="H42" t="str">
-        <f>"$this-&gt;"&amp;C2&amp;" = $row['"&amp;C2&amp;"'];"</f>
+        <f t="shared" si="42"/>
         <v>$this-&gt;title = $row['title'];</v>
       </c>
       <c r="L42" t="str">
-        <f>"$member-&gt;"&amp;C2&amp;" = $data-&gt;"&amp;C2&amp;";"</f>
-        <v>$member-&gt;title = $data-&gt;title;</v>
+        <f t="shared" ref="L42:L74" si="43">"$item-&gt;"&amp;C2&amp;" = $data-&gt;"&amp;C2&amp;";"</f>
+        <v>$item-&gt;title = $data-&gt;title;</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
-        <f>C3&amp;" = :"&amp;C3&amp;","</f>
+        <f t="shared" si="40"/>
         <v>businessname = :businessname,</v>
       </c>
       <c r="D43" t="str">
-        <f>""""&amp;C3&amp;""" =&gt; $member-&gt;"&amp;C3&amp;","</f>
+        <f t="shared" si="41"/>
         <v>"businessname" =&gt; $member-&gt;businessname,</v>
       </c>
       <c r="H43" t="str">
-        <f>"$this-&gt;"&amp;C3&amp;" = $row['"&amp;C3&amp;"'];"</f>
+        <f t="shared" si="42"/>
         <v>$this-&gt;businessname = $row['businessname'];</v>
       </c>
       <c r="L43" t="str">
-        <f>"$member-&gt;"&amp;C3&amp;" = $data-&gt;"&amp;C3&amp;";"</f>
-        <v>$member-&gt;businessname = $data-&gt;businessname;</v>
+        <f t="shared" si="43"/>
+        <v>$item-&gt;businessname = $data-&gt;businessname;</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
-        <f>C4&amp;" = :"&amp;C4&amp;","</f>
+        <f t="shared" si="40"/>
         <v>bankpayerref = :bankpayerref,</v>
       </c>
       <c r="D44" t="str">
-        <f>""""&amp;C4&amp;""" =&gt; $member-&gt;"&amp;C4&amp;","</f>
+        <f t="shared" si="41"/>
         <v>"bankpayerref" =&gt; $member-&gt;bankpayerref,</v>
       </c>
       <c r="H44" t="str">
-        <f>"$this-&gt;"&amp;C4&amp;" = $row['"&amp;C4&amp;"'];"</f>
+        <f t="shared" si="42"/>
         <v>$this-&gt;bankpayerref = $row['bankpayerref'];</v>
       </c>
       <c r="L44" t="str">
-        <f>"$member-&gt;"&amp;C4&amp;" = $data-&gt;"&amp;C4&amp;";"</f>
-        <v>$member-&gt;bankpayerref = $data-&gt;bankpayerref;</v>
+        <f t="shared" si="43"/>
+        <v>$item-&gt;bankpayerref = $data-&gt;bankpayerref;</v>
       </c>
       <c r="R44" t="str">
         <f>S44&amp;","</f>
         <v>bankpayerref,</v>
       </c>
       <c r="S44" t="str">
-        <f>C4</f>
+        <f t="shared" ref="S44:S49" si="44">C4</f>
         <v>bankpayerref</v>
       </c>
       <c r="T44" s="1" t="str">
@@ -2073,193 +2073,193 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
-        <f>C5&amp;" = :"&amp;C5&amp;","</f>
+        <f t="shared" si="40"/>
         <v>note = :note,</v>
       </c>
       <c r="D45" t="str">
-        <f>""""&amp;C5&amp;""" =&gt; $member-&gt;"&amp;C5&amp;","</f>
+        <f t="shared" si="41"/>
         <v>"note" =&gt; $member-&gt;note,</v>
       </c>
       <c r="H45" t="str">
-        <f>"$this-&gt;"&amp;C5&amp;" = $row['"&amp;C5&amp;"'];"</f>
+        <f t="shared" si="42"/>
         <v>$this-&gt;note = $row['note'];</v>
       </c>
       <c r="L45" t="str">
-        <f>"$member-&gt;"&amp;C5&amp;" = $data-&gt;"&amp;C5&amp;";"</f>
-        <v>$member-&gt;note = $data-&gt;note;</v>
+        <f t="shared" si="43"/>
+        <v>$item-&gt;note = $data-&gt;note;</v>
       </c>
       <c r="R45" t="str">
-        <f t="shared" ref="R45:R68" si="40">S45&amp;","</f>
+        <f t="shared" ref="R45:R51" si="45">S45&amp;","</f>
         <v>note,</v>
       </c>
       <c r="S45" t="str">
-        <f>C5</f>
+        <f t="shared" si="44"/>
         <v>note</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" ref="T45:T68" si="41">",SUM("&amp;S45&amp;") as sum_"&amp;S45</f>
+        <f t="shared" ref="T45:T51" si="46">",SUM("&amp;S45&amp;") as sum_"&amp;S45</f>
         <v>,SUM(note) as sum_note</v>
       </c>
       <c r="U45" s="1" t="str">
-        <f t="shared" ref="U45:U68" si="42">",AVG("&amp;S45&amp;") as avg_"&amp;S45</f>
+        <f t="shared" ref="U45:U51" si="47">",AVG("&amp;S45&amp;") as avg_"&amp;S45</f>
         <v>,AVG(note) as avg_note</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
-        <f>C6&amp;" = :"&amp;C6&amp;","</f>
+        <f t="shared" si="40"/>
         <v>addressfirstline = :addressfirstline,</v>
       </c>
       <c r="D46" t="str">
-        <f>""""&amp;C6&amp;""" =&gt; $member-&gt;"&amp;C6&amp;","</f>
+        <f t="shared" si="41"/>
         <v>"addressfirstline" =&gt; $member-&gt;addressfirstline,</v>
       </c>
       <c r="H46" t="str">
-        <f>"$this-&gt;"&amp;C6&amp;" = $row['"&amp;C6&amp;"'];"</f>
+        <f t="shared" si="42"/>
         <v>$this-&gt;addressfirstline = $row['addressfirstline'];</v>
       </c>
       <c r="L46" t="str">
-        <f>"$member-&gt;"&amp;C6&amp;" = $data-&gt;"&amp;C6&amp;";"</f>
-        <v>$member-&gt;addressfirstline = $data-&gt;addressfirstline;</v>
+        <f t="shared" si="43"/>
+        <v>$item-&gt;addressfirstline = $data-&gt;addressfirstline;</v>
       </c>
       <c r="R46" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>addressfirstline,</v>
       </c>
       <c r="S46" t="str">
-        <f>C6</f>
+        <f t="shared" si="44"/>
         <v>addressfirstline</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>,SUM(addressfirstline) as sum_addressfirstline</v>
       </c>
       <c r="U46" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>,AVG(addressfirstline) as avg_addressfirstline</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
-        <f>C7&amp;" = :"&amp;C7&amp;","</f>
+        <f t="shared" si="40"/>
         <v>addresssecondline = :addresssecondline,</v>
       </c>
       <c r="D47" t="str">
-        <f>""""&amp;C7&amp;""" =&gt; $member-&gt;"&amp;C7&amp;","</f>
+        <f t="shared" si="41"/>
         <v>"addresssecondline" =&gt; $member-&gt;addresssecondline,</v>
       </c>
       <c r="H47" t="str">
-        <f>"$this-&gt;"&amp;C7&amp;" = $row['"&amp;C7&amp;"'];"</f>
+        <f t="shared" si="42"/>
         <v>$this-&gt;addresssecondline = $row['addresssecondline'];</v>
       </c>
       <c r="L47" t="str">
-        <f>"$member-&gt;"&amp;C7&amp;" = $data-&gt;"&amp;C7&amp;";"</f>
-        <v>$member-&gt;addresssecondline = $data-&gt;addresssecondline;</v>
+        <f t="shared" si="43"/>
+        <v>$item-&gt;addresssecondline = $data-&gt;addresssecondline;</v>
       </c>
       <c r="R47" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>addresssecondline,</v>
       </c>
       <c r="S47" t="str">
-        <f>C7</f>
+        <f t="shared" si="44"/>
         <v>addresssecondline</v>
       </c>
       <c r="T47" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>,SUM(addresssecondline) as sum_addresssecondline</v>
       </c>
       <c r="U47" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>,AVG(addresssecondline) as avg_addresssecondline</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
-        <f>C8&amp;" = :"&amp;C8&amp;","</f>
+        <f t="shared" si="40"/>
         <v>city = :city,</v>
       </c>
       <c r="D48" t="str">
-        <f>""""&amp;C8&amp;""" =&gt; $member-&gt;"&amp;C8&amp;","</f>
+        <f t="shared" si="41"/>
         <v>"city" =&gt; $member-&gt;city,</v>
       </c>
       <c r="H48" t="str">
-        <f>"$this-&gt;"&amp;C8&amp;" = $row['"&amp;C8&amp;"'];"</f>
+        <f t="shared" si="42"/>
         <v>$this-&gt;city = $row['city'];</v>
       </c>
       <c r="L48" t="str">
-        <f>"$member-&gt;"&amp;C8&amp;" = $data-&gt;"&amp;C8&amp;";"</f>
-        <v>$member-&gt;city = $data-&gt;city;</v>
+        <f t="shared" si="43"/>
+        <v>$item-&gt;city = $data-&gt;city;</v>
       </c>
       <c r="R48" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>city,</v>
       </c>
       <c r="S48" t="str">
-        <f>C8</f>
+        <f t="shared" si="44"/>
         <v>city</v>
       </c>
       <c r="T48" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>,SUM(city) as sum_city</v>
       </c>
       <c r="U48" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>,AVG(city) as avg_city</v>
       </c>
     </row>
     <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
-        <f>C9&amp;" = :"&amp;C9&amp;","</f>
+        <f t="shared" si="40"/>
         <v>county = :county,</v>
       </c>
       <c r="D49" t="str">
-        <f>""""&amp;C9&amp;""" =&gt; $member-&gt;"&amp;C9&amp;","</f>
+        <f t="shared" si="41"/>
         <v>"county" =&gt; $member-&gt;county,</v>
       </c>
       <c r="H49" t="str">
-        <f>"$this-&gt;"&amp;C9&amp;" = $row['"&amp;C9&amp;"'];"</f>
+        <f t="shared" si="42"/>
         <v>$this-&gt;county = $row['county'];</v>
       </c>
       <c r="L49" t="str">
-        <f>"$member-&gt;"&amp;C9&amp;" = $data-&gt;"&amp;C9&amp;";"</f>
-        <v>$member-&gt;county = $data-&gt;county;</v>
+        <f t="shared" si="43"/>
+        <v>$item-&gt;county = $data-&gt;county;</v>
       </c>
       <c r="R49" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>county,</v>
       </c>
       <c r="S49" t="str">
-        <f>C9</f>
+        <f t="shared" si="44"/>
         <v>county</v>
       </c>
       <c r="T49" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>,SUM(county) as sum_county</v>
       </c>
       <c r="U49" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>,AVG(county) as avg_county</v>
       </c>
     </row>
     <row r="50" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
-        <f>C10&amp;" = :"&amp;C10&amp;","</f>
+        <f t="shared" si="40"/>
         <v>postcode = :postcode,</v>
       </c>
       <c r="D50" t="str">
-        <f>""""&amp;C10&amp;""" =&gt; $member-&gt;"&amp;C10&amp;","</f>
+        <f t="shared" si="41"/>
         <v>"postcode" =&gt; $member-&gt;postcode,</v>
       </c>
       <c r="H50" t="str">
-        <f>"$this-&gt;"&amp;C10&amp;" = $row['"&amp;C10&amp;"'];"</f>
+        <f t="shared" si="42"/>
         <v>$this-&gt;postcode = $row['postcode'];</v>
       </c>
       <c r="L50" t="str">
-        <f>"$member-&gt;"&amp;C10&amp;" = $data-&gt;"&amp;C10&amp;";"</f>
-        <v>$member-&gt;postcode = $data-&gt;postcode;</v>
+        <f t="shared" si="43"/>
+        <v>$item-&gt;postcode = $data-&gt;postcode;</v>
       </c>
       <c r="R50" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>country,</v>
       </c>
       <c r="S50" t="str">
@@ -2267,33 +2267,33 @@
         <v>country</v>
       </c>
       <c r="T50" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>,SUM(country) as sum_country</v>
       </c>
       <c r="U50" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>,AVG(country) as avg_country</v>
       </c>
     </row>
     <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
-        <f>C11&amp;" = :"&amp;C11&amp;","</f>
+        <f t="shared" si="40"/>
         <v>country = :country,</v>
       </c>
       <c r="D51" t="str">
-        <f>""""&amp;C11&amp;""" =&gt; $member-&gt;"&amp;C11&amp;","</f>
+        <f t="shared" si="41"/>
         <v>"country" =&gt; $member-&gt;country,</v>
       </c>
       <c r="H51" t="str">
-        <f>"$this-&gt;"&amp;C11&amp;" = $row['"&amp;C11&amp;"'];"</f>
+        <f t="shared" si="42"/>
         <v>$this-&gt;country = $row['country'];</v>
       </c>
       <c r="L51" t="str">
-        <f>"$member-&gt;"&amp;C11&amp;" = $data-&gt;"&amp;C11&amp;";"</f>
-        <v>$member-&gt;country = $data-&gt;country;</v>
+        <f t="shared" si="43"/>
+        <v>$item-&gt;country = $data-&gt;country;</v>
       </c>
       <c r="R51" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>email1,</v>
       </c>
       <c r="S51" t="str">
@@ -2301,793 +2301,793 @@
         <v>email1</v>
       </c>
       <c r="T51" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>,SUM(email1) as sum_email1</v>
       </c>
       <c r="U51" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>,AVG(email1) as avg_email1</v>
       </c>
     </row>
     <row r="52" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
-        <f t="shared" ref="B52:B75" si="43">C12&amp;" = :"&amp;C12&amp;","</f>
+        <f t="shared" ref="B52:B74" si="48">C12&amp;" = :"&amp;C12&amp;","</f>
         <v>area = :area,</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" ref="D52:D75" si="44">""""&amp;C12&amp;""" =&gt; $member-&gt;"&amp;C12&amp;","</f>
+        <f t="shared" ref="D52:D74" si="49">""""&amp;C12&amp;""" =&gt; $member-&gt;"&amp;C12&amp;","</f>
         <v>"area" =&gt; $member-&gt;area,</v>
       </c>
       <c r="H52" t="str">
-        <f t="shared" ref="H52:H75" si="45">"$this-&gt;"&amp;C12&amp;" = $row['"&amp;C12&amp;"'];"</f>
+        <f t="shared" ref="H52:H74" si="50">"$this-&gt;"&amp;C12&amp;" = $row['"&amp;C12&amp;"'];"</f>
         <v>$this-&gt;area = $row['area'];</v>
       </c>
       <c r="L52" t="str">
-        <f t="shared" ref="L52:L75" si="46">"$member-&gt;"&amp;C12&amp;" = $data-&gt;"&amp;C12&amp;";"</f>
-        <v>$member-&gt;area = $data-&gt;area;</v>
+        <f t="shared" si="43"/>
+        <v>$item-&gt;area = $data-&gt;area;</v>
       </c>
       <c r="R52" t="str">
-        <f t="shared" ref="R52:R75" si="47">S52&amp;","</f>
+        <f t="shared" ref="R52:R74" si="51">S52&amp;","</f>
         <v>phone1,</v>
       </c>
       <c r="S52" t="str">
-        <f t="shared" ref="S52:S75" si="48">C14</f>
+        <f t="shared" ref="S52:S74" si="52">C14</f>
         <v>phone1</v>
       </c>
       <c r="T52" t="str">
-        <f t="shared" ref="T52:T75" si="49">",SUM("&amp;S52&amp;") as sum_"&amp;S52</f>
+        <f t="shared" ref="T52:T74" si="53">",SUM("&amp;S52&amp;") as sum_"&amp;S52</f>
         <v>,SUM(phone1) as sum_phone1</v>
       </c>
       <c r="U52" s="1" t="str">
-        <f t="shared" ref="U52:U75" si="50">",AVG("&amp;S52&amp;") as avg_"&amp;S52</f>
+        <f t="shared" ref="U52:U74" si="54">",AVG("&amp;S52&amp;") as avg_"&amp;S52</f>
         <v>,AVG(phone1) as avg_phone1</v>
       </c>
     </row>
     <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
+        <f t="shared" si="48"/>
+        <v>email1 = :email1,</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="49"/>
+        <v>"email1" =&gt; $member-&gt;email1,</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;email1 = $row['email1'];</v>
+      </c>
+      <c r="L53" t="str">
         <f t="shared" si="43"/>
-        <v>email1 = :email1,</v>
-      </c>
-      <c r="D53" t="str">
-        <f t="shared" si="44"/>
-        <v>"email1" =&gt; $member-&gt;email1,</v>
-      </c>
-      <c r="H53" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;email1 = $row['email1'];</v>
-      </c>
-      <c r="L53" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;email1 = $data-&gt;email1;</v>
+        <v>$item-&gt;email1 = $data-&gt;email1;</v>
       </c>
       <c r="R53" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>addressfirstline2,</v>
       </c>
       <c r="S53" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>addressfirstline2</v>
       </c>
       <c r="T53" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(addressfirstline2) as sum_addressfirstline2</v>
       </c>
       <c r="U53" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(addressfirstline2) as avg_addressfirstline2</v>
       </c>
     </row>
     <row r="54" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
+        <f t="shared" si="48"/>
+        <v>phone1 = :phone1,</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="49"/>
+        <v>"phone1" =&gt; $member-&gt;phone1,</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;phone1 = $row['phone1'];</v>
+      </c>
+      <c r="L54" t="str">
         <f t="shared" si="43"/>
-        <v>phone1 = :phone1,</v>
-      </c>
-      <c r="D54" t="str">
-        <f t="shared" si="44"/>
-        <v>"phone1" =&gt; $member-&gt;phone1,</v>
-      </c>
-      <c r="H54" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;phone1 = $row['phone1'];</v>
-      </c>
-      <c r="L54" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;phone1 = $data-&gt;phone1;</v>
+        <v>$item-&gt;phone1 = $data-&gt;phone1;</v>
       </c>
       <c r="R54" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>addresssecondline2,</v>
       </c>
       <c r="S54" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>addresssecondline2</v>
       </c>
       <c r="T54" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(addresssecondline2) as sum_addresssecondline2</v>
       </c>
       <c r="U54" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(addresssecondline2) as avg_addresssecondline2</v>
       </c>
     </row>
     <row r="55" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
+        <f t="shared" si="48"/>
+        <v>addressfirstline2 = :addressfirstline2,</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="49"/>
+        <v>"addressfirstline2" =&gt; $member-&gt;addressfirstline2,</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;addressfirstline2 = $row['addressfirstline2'];</v>
+      </c>
+      <c r="L55" t="str">
         <f t="shared" si="43"/>
-        <v>addressfirstline2 = :addressfirstline2,</v>
-      </c>
-      <c r="D55" t="str">
-        <f t="shared" si="44"/>
-        <v>"addressfirstline2" =&gt; $member-&gt;addressfirstline2,</v>
-      </c>
-      <c r="H55" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;addressfirstline2 = $row['addressfirstline2'];</v>
-      </c>
-      <c r="L55" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;addressfirstline2 = $data-&gt;addressfirstline2;</v>
+        <v>$item-&gt;addressfirstline2 = $data-&gt;addressfirstline2;</v>
       </c>
       <c r="R55" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>city2,</v>
       </c>
       <c r="S55" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>city2</v>
       </c>
       <c r="T55" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(city2) as sum_city2</v>
       </c>
       <c r="U55" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(city2) as avg_city2</v>
       </c>
     </row>
     <row r="56" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
+        <f t="shared" si="48"/>
+        <v>addresssecondline2 = :addresssecondline2,</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="49"/>
+        <v>"addresssecondline2" =&gt; $member-&gt;addresssecondline2,</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;addresssecondline2 = $row['addresssecondline2'];</v>
+      </c>
+      <c r="L56" t="str">
         <f t="shared" si="43"/>
-        <v>addresssecondline2 = :addresssecondline2,</v>
-      </c>
-      <c r="D56" t="str">
-        <f t="shared" si="44"/>
-        <v>"addresssecondline2" =&gt; $member-&gt;addresssecondline2,</v>
-      </c>
-      <c r="H56" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;addresssecondline2 = $row['addresssecondline2'];</v>
-      </c>
-      <c r="L56" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;addresssecondline2 = $data-&gt;addresssecondline2;</v>
+        <v>$item-&gt;addresssecondline2 = $data-&gt;addresssecondline2;</v>
       </c>
       <c r="R56" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>county2,</v>
       </c>
       <c r="S56" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>county2</v>
       </c>
       <c r="T56" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(county2) as sum_county2</v>
       </c>
       <c r="U56" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(county2) as avg_county2</v>
       </c>
     </row>
     <row r="57" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
+        <f t="shared" si="48"/>
+        <v>city2 = :city2,</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="49"/>
+        <v>"city2" =&gt; $member-&gt;city2,</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;city2 = $row['city2'];</v>
+      </c>
+      <c r="L57" t="str">
         <f t="shared" si="43"/>
-        <v>city2 = :city2,</v>
-      </c>
-      <c r="D57" t="str">
-        <f t="shared" si="44"/>
-        <v>"city2" =&gt; $member-&gt;city2,</v>
-      </c>
-      <c r="H57" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;city2 = $row['city2'];</v>
-      </c>
-      <c r="L57" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;city2 = $data-&gt;city2;</v>
+        <v>$item-&gt;city2 = $data-&gt;city2;</v>
       </c>
       <c r="R57" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>postcode2,</v>
       </c>
       <c r="S57" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>postcode2</v>
       </c>
       <c r="T57" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(postcode2) as sum_postcode2</v>
       </c>
       <c r="U57" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(postcode2) as avg_postcode2</v>
       </c>
     </row>
     <row r="58" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
+        <f t="shared" si="48"/>
+        <v>county2 = :county2,</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="49"/>
+        <v>"county2" =&gt; $member-&gt;county2,</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;county2 = $row['county2'];</v>
+      </c>
+      <c r="L58" t="str">
         <f t="shared" si="43"/>
-        <v>county2 = :county2,</v>
-      </c>
-      <c r="D58" t="str">
-        <f t="shared" si="44"/>
-        <v>"county2" =&gt; $member-&gt;county2,</v>
-      </c>
-      <c r="H58" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;county2 = $row['county2'];</v>
-      </c>
-      <c r="L58" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;county2 = $data-&gt;county2;</v>
+        <v>$item-&gt;county2 = $data-&gt;county2;</v>
       </c>
       <c r="R58" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>country2,</v>
       </c>
       <c r="S58" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>country2</v>
       </c>
       <c r="T58" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(country2) as sum_country2</v>
       </c>
       <c r="U58" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(country2) as avg_country2</v>
       </c>
     </row>
     <row r="59" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B59" t="str">
+        <f t="shared" si="48"/>
+        <v>postcode2 = :postcode2,</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="49"/>
+        <v>"postcode2" =&gt; $member-&gt;postcode2,</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;postcode2 = $row['postcode2'];</v>
+      </c>
+      <c r="L59" t="str">
         <f t="shared" si="43"/>
-        <v>postcode2 = :postcode2,</v>
-      </c>
-      <c r="D59" t="str">
-        <f t="shared" si="44"/>
-        <v>"postcode2" =&gt; $member-&gt;postcode2,</v>
-      </c>
-      <c r="H59" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;postcode2 = $row['postcode2'];</v>
-      </c>
-      <c r="L59" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;postcode2 = $data-&gt;postcode2;</v>
+        <v>$item-&gt;postcode2 = $data-&gt;postcode2;</v>
       </c>
       <c r="R59" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>email2,</v>
       </c>
       <c r="S59" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>email2</v>
       </c>
       <c r="T59" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(email2) as sum_email2</v>
       </c>
       <c r="U59" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(email2) as avg_email2</v>
       </c>
     </row>
     <row r="60" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B60" t="str">
+        <f t="shared" si="48"/>
+        <v>country2 = :country2,</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="49"/>
+        <v>"country2" =&gt; $member-&gt;country2,</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;country2 = $row['country2'];</v>
+      </c>
+      <c r="L60" t="str">
         <f t="shared" si="43"/>
-        <v>country2 = :country2,</v>
-      </c>
-      <c r="D60" t="str">
-        <f t="shared" si="44"/>
-        <v>"country2" =&gt; $member-&gt;country2,</v>
-      </c>
-      <c r="H60" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;country2 = $row['country2'];</v>
-      </c>
-      <c r="L60" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;country2 = $data-&gt;country2;</v>
+        <v>$item-&gt;country2 = $data-&gt;country2;</v>
       </c>
       <c r="R60" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>phone2,</v>
       </c>
       <c r="S60" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>phone2</v>
       </c>
       <c r="T60" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(phone2) as sum_phone2</v>
       </c>
       <c r="U60" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(phone2) as avg_phone2</v>
       </c>
     </row>
     <row r="61" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B61" t="str">
+        <f t="shared" si="48"/>
+        <v>email2 = :email2,</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="49"/>
+        <v>"email2" =&gt; $member-&gt;email2,</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;email2 = $row['email2'];</v>
+      </c>
+      <c r="L61" t="str">
         <f t="shared" si="43"/>
-        <v>email2 = :email2,</v>
-      </c>
-      <c r="D61" t="str">
-        <f t="shared" si="44"/>
-        <v>"email2" =&gt; $member-&gt;email2,</v>
-      </c>
-      <c r="H61" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;email2 = $row['email2'];</v>
-      </c>
-      <c r="L61" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;email2 = $data-&gt;email2;</v>
+        <v>$item-&gt;email2 = $data-&gt;email2;</v>
       </c>
       <c r="R61" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>statusID,</v>
       </c>
       <c r="S61" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>statusID</v>
       </c>
       <c r="T61" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(statusID) as sum_statusID</v>
       </c>
       <c r="U61" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(statusID) as avg_statusID</v>
       </c>
     </row>
     <row r="62" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B62" t="str">
+        <f t="shared" si="48"/>
+        <v>phone2 = :phone2,</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="49"/>
+        <v>"phone2" =&gt; $member-&gt;phone2,</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;phone2 = $row['phone2'];</v>
+      </c>
+      <c r="L62" t="str">
         <f t="shared" si="43"/>
-        <v>phone2 = :phone2,</v>
-      </c>
-      <c r="D62" t="str">
-        <f t="shared" si="44"/>
-        <v>"phone2" =&gt; $member-&gt;phone2,</v>
-      </c>
-      <c r="H62" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;phone2 = $row['phone2'];</v>
-      </c>
-      <c r="L62" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;phone2 = $data-&gt;phone2;</v>
+        <v>$item-&gt;phone2 = $data-&gt;phone2;</v>
       </c>
       <c r="R62" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>expirydate,</v>
       </c>
       <c r="S62" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>expirydate</v>
       </c>
       <c r="T62" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(expirydate) as sum_expirydate</v>
       </c>
       <c r="U62" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(expirydate) as avg_expirydate</v>
       </c>
     </row>
     <row r="63" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
+        <f t="shared" si="48"/>
+        <v>statusID = :statusID,</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="49"/>
+        <v>"statusID" =&gt; $member-&gt;statusID,</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;statusID = $row['statusID'];</v>
+      </c>
+      <c r="L63" t="str">
         <f t="shared" si="43"/>
-        <v>statusID = :statusID,</v>
-      </c>
-      <c r="D63" t="str">
-        <f t="shared" si="44"/>
-        <v>"statusID" =&gt; $member-&gt;statusID,</v>
-      </c>
-      <c r="H63" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;statusID = $row['statusID'];</v>
-      </c>
-      <c r="L63" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;statusID = $data-&gt;statusID;</v>
+        <v>$item-&gt;statusID = $data-&gt;statusID;</v>
       </c>
       <c r="R63" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>joindate,</v>
       </c>
       <c r="S63" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>joindate</v>
       </c>
       <c r="T63" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(joindate) as sum_joindate</v>
       </c>
       <c r="U63" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(joindate) as avg_joindate</v>
       </c>
     </row>
     <row r="64" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
+        <f t="shared" si="48"/>
+        <v>expirydate = :expirydate,</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="49"/>
+        <v>"expirydate" =&gt; $member-&gt;expirydate,</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;expirydate = $row['expirydate'];</v>
+      </c>
+      <c r="L64" t="str">
         <f t="shared" si="43"/>
-        <v>expirydate = :expirydate,</v>
-      </c>
-      <c r="D64" t="str">
-        <f t="shared" si="44"/>
-        <v>"expirydate" =&gt; $member-&gt;expirydate,</v>
-      </c>
-      <c r="H64" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;expirydate = $row['expirydate'];</v>
-      </c>
-      <c r="L64" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;expirydate = $data-&gt;expirydate;</v>
+        <v>$item-&gt;expirydate = $data-&gt;expirydate;</v>
       </c>
       <c r="R64" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>updatedate,</v>
       </c>
       <c r="S64" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>updatedate</v>
       </c>
       <c r="T64" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(updatedate) as sum_updatedate</v>
       </c>
       <c r="U64" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(updatedate) as avg_updatedate</v>
       </c>
     </row>
     <row r="65" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B65" t="str">
+        <f t="shared" si="48"/>
+        <v>joindate = :joindate,</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="49"/>
+        <v>"joindate" =&gt; $member-&gt;joindate,</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;joindate = $row['joindate'];</v>
+      </c>
+      <c r="L65" t="str">
         <f t="shared" si="43"/>
-        <v>joindate = :joindate,</v>
-      </c>
-      <c r="D65" t="str">
-        <f t="shared" si="44"/>
-        <v>"joindate" =&gt; $member-&gt;joindate,</v>
-      </c>
-      <c r="H65" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;joindate = $row['joindate'];</v>
-      </c>
-      <c r="L65" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;joindate = $data-&gt;joindate;</v>
+        <v>$item-&gt;joindate = $data-&gt;joindate;</v>
       </c>
       <c r="R65" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>deletedate,</v>
       </c>
       <c r="S65" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>deletedate</v>
       </c>
       <c r="T65" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(deletedate) as sum_deletedate</v>
       </c>
       <c r="U65" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(deletedate) as avg_deletedate</v>
       </c>
     </row>
     <row r="66" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B66" t="str">
+        <f t="shared" si="48"/>
+        <v>updatedate = :updatedate,</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="49"/>
+        <v>"updatedate" =&gt; $member-&gt;updatedate,</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;updatedate = $row['updatedate'];</v>
+      </c>
+      <c r="L66" t="str">
         <f t="shared" si="43"/>
-        <v>updatedate = :updatedate,</v>
-      </c>
-      <c r="D66" t="str">
-        <f t="shared" si="44"/>
-        <v>"updatedate" =&gt; $member-&gt;updatedate,</v>
-      </c>
-      <c r="H66" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;updatedate = $row['updatedate'];</v>
-      </c>
-      <c r="L66" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;updatedate = $data-&gt;updatedate;</v>
+        <v>$item-&gt;updatedate = $data-&gt;updatedate;</v>
       </c>
       <c r="R66" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>repeatpayment,</v>
       </c>
       <c r="S66" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>repeatpayment</v>
       </c>
       <c r="T66" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(repeatpayment) as sum_repeatpayment</v>
       </c>
       <c r="U66" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(repeatpayment) as avg_repeatpayment</v>
       </c>
     </row>
     <row r="67" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B67" t="str">
+        <f t="shared" si="48"/>
+        <v>deletedate = :deletedate,</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="49"/>
+        <v>"deletedate" =&gt; $member-&gt;deletedate,</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;deletedate = $row['deletedate'];</v>
+      </c>
+      <c r="L67" t="str">
         <f t="shared" si="43"/>
-        <v>deletedate = :deletedate,</v>
-      </c>
-      <c r="D67" t="str">
-        <f t="shared" si="44"/>
-        <v>"deletedate" =&gt; $member-&gt;deletedate,</v>
-      </c>
-      <c r="H67" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;deletedate = $row['deletedate'];</v>
-      </c>
-      <c r="L67" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;deletedate = $data-&gt;deletedate;</v>
+        <v>$item-&gt;deletedate = $data-&gt;deletedate;</v>
       </c>
       <c r="R67" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>recurringpayment,</v>
       </c>
       <c r="S67" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>recurringpayment</v>
       </c>
       <c r="T67" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(recurringpayment) as sum_recurringpayment</v>
       </c>
       <c r="U67" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(recurringpayment) as avg_recurringpayment</v>
       </c>
     </row>
     <row r="68" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B68" t="str">
+        <f t="shared" si="48"/>
+        <v>repeatpayment = :repeatpayment,</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="49"/>
+        <v>"repeatpayment" =&gt; $member-&gt;repeatpayment,</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;repeatpayment = $row['repeatpayment'];</v>
+      </c>
+      <c r="L68" t="str">
         <f t="shared" si="43"/>
-        <v>repeatpayment = :repeatpayment,</v>
-      </c>
-      <c r="D68" t="str">
-        <f t="shared" si="44"/>
-        <v>"repeatpayment" =&gt; $member-&gt;repeatpayment,</v>
-      </c>
-      <c r="H68" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;repeatpayment = $row['repeatpayment'];</v>
-      </c>
-      <c r="L68" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;repeatpayment = $data-&gt;repeatpayment;</v>
+        <v>$item-&gt;repeatpayment = $data-&gt;repeatpayment;</v>
       </c>
       <c r="R68" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>username,</v>
       </c>
       <c r="S68" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>username</v>
       </c>
       <c r="T68" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(username) as sum_username</v>
       </c>
       <c r="U68" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(username) as avg_username</v>
       </c>
     </row>
     <row r="69" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B69" t="str">
+        <f t="shared" si="48"/>
+        <v>recurringpayment = :recurringpayment,</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="49"/>
+        <v>"recurringpayment" =&gt; $member-&gt;recurringpayment,</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;recurringpayment = $row['recurringpayment'];</v>
+      </c>
+      <c r="L69" t="str">
         <f t="shared" si="43"/>
-        <v>recurringpayment = :recurringpayment,</v>
-      </c>
-      <c r="D69" t="str">
-        <f t="shared" si="44"/>
-        <v>"recurringpayment" =&gt; $member-&gt;recurringpayment,</v>
-      </c>
-      <c r="H69" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;recurringpayment = $row['recurringpayment'];</v>
-      </c>
-      <c r="L69" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;recurringpayment = $data-&gt;recurringpayment;</v>
+        <v>$item-&gt;recurringpayment = $data-&gt;recurringpayment;</v>
       </c>
       <c r="R69" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>gdpr_email,</v>
       </c>
       <c r="S69" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>gdpr_email</v>
       </c>
       <c r="T69" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(gdpr_email) as sum_gdpr_email</v>
       </c>
       <c r="U69" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(gdpr_email) as avg_gdpr_email</v>
       </c>
     </row>
     <row r="70" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B70" t="str">
+        <f t="shared" si="48"/>
+        <v>username = :username,</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="49"/>
+        <v>"username" =&gt; $member-&gt;username,</v>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;username = $row['username'];</v>
+      </c>
+      <c r="L70" t="str">
         <f t="shared" si="43"/>
-        <v>username = :username,</v>
-      </c>
-      <c r="D70" t="str">
-        <f t="shared" si="44"/>
-        <v>"username" =&gt; $member-&gt;username,</v>
-      </c>
-      <c r="H70" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;username = $row['username'];</v>
-      </c>
-      <c r="L70" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;username = $data-&gt;username;</v>
+        <v>$item-&gt;username = $data-&gt;username;</v>
       </c>
       <c r="R70" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>gdpr_tel,</v>
       </c>
       <c r="S70" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>gdpr_tel</v>
       </c>
       <c r="T70" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(gdpr_tel) as sum_gdpr_tel</v>
       </c>
       <c r="U70" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(gdpr_tel) as avg_gdpr_tel</v>
       </c>
     </row>
     <row r="71" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B71" t="str">
+        <f t="shared" si="48"/>
+        <v>gdpr_email = :gdpr_email,</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="49"/>
+        <v>"gdpr_email" =&gt; $member-&gt;gdpr_email,</v>
+      </c>
+      <c r="H71" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;gdpr_email = $row['gdpr_email'];</v>
+      </c>
+      <c r="L71" t="str">
         <f t="shared" si="43"/>
-        <v>gdpr_email = :gdpr_email,</v>
-      </c>
-      <c r="D71" t="str">
-        <f t="shared" si="44"/>
-        <v>"gdpr_email" =&gt; $member-&gt;gdpr_email,</v>
-      </c>
-      <c r="H71" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;gdpr_email = $row['gdpr_email'];</v>
-      </c>
-      <c r="L71" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;gdpr_email = $data-&gt;gdpr_email;</v>
+        <v>$item-&gt;gdpr_email = $data-&gt;gdpr_email;</v>
       </c>
       <c r="R71" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>gdpr_address,</v>
       </c>
       <c r="S71" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>gdpr_address</v>
       </c>
       <c r="T71" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(gdpr_address) as sum_gdpr_address</v>
       </c>
       <c r="U71" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(gdpr_address) as avg_gdpr_address</v>
       </c>
     </row>
     <row r="72" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B72" t="str">
+        <f t="shared" si="48"/>
+        <v>gdpr_tel = :gdpr_tel,</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="49"/>
+        <v>"gdpr_tel" =&gt; $member-&gt;gdpr_tel,</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;gdpr_tel = $row['gdpr_tel'];</v>
+      </c>
+      <c r="L72" t="str">
         <f t="shared" si="43"/>
-        <v>gdpr_tel = :gdpr_tel,</v>
-      </c>
-      <c r="D72" t="str">
-        <f t="shared" si="44"/>
-        <v>"gdpr_tel" =&gt; $member-&gt;gdpr_tel,</v>
-      </c>
-      <c r="H72" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;gdpr_tel = $row['gdpr_tel'];</v>
-      </c>
-      <c r="L72" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;gdpr_tel = $data-&gt;gdpr_tel;</v>
+        <v>$item-&gt;gdpr_tel = $data-&gt;gdpr_tel;</v>
       </c>
       <c r="R72" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>gdpr_sm,</v>
       </c>
       <c r="S72" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>gdpr_sm</v>
       </c>
       <c r="T72" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(gdpr_sm) as sum_gdpr_sm</v>
       </c>
       <c r="U72" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(gdpr_sm) as avg_gdpr_sm</v>
       </c>
     </row>
     <row r="73" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B73" t="str">
+        <f t="shared" si="48"/>
+        <v>gdpr_address = :gdpr_address,</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="49"/>
+        <v>"gdpr_address" =&gt; $member-&gt;gdpr_address,</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;gdpr_address = $row['gdpr_address'];</v>
+      </c>
+      <c r="L73" t="str">
         <f t="shared" si="43"/>
-        <v>gdpr_address = :gdpr_address,</v>
-      </c>
-      <c r="D73" t="str">
-        <f t="shared" si="44"/>
-        <v>"gdpr_address" =&gt; $member-&gt;gdpr_address,</v>
-      </c>
-      <c r="H73" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;gdpr_address = $row['gdpr_address'];</v>
-      </c>
-      <c r="L73" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;gdpr_address = $data-&gt;gdpr_address;</v>
+        <v>$item-&gt;gdpr_address = $data-&gt;gdpr_address;</v>
       </c>
       <c r="R73" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>0,</v>
       </c>
       <c r="S73">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="T73" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(0) as sum_0</v>
       </c>
       <c r="U73" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(0) as avg_0</v>
       </c>
     </row>
     <row r="74" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B74" t="str">
+        <f t="shared" si="48"/>
+        <v>gdpr_sm = :gdpr_sm,</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="49"/>
+        <v>"gdpr_sm" =&gt; $member-&gt;gdpr_sm,</v>
+      </c>
+      <c r="H74" t="str">
+        <f t="shared" si="50"/>
+        <v>$this-&gt;gdpr_sm = $row['gdpr_sm'];</v>
+      </c>
+      <c r="L74" t="str">
         <f t="shared" si="43"/>
-        <v>gdpr_sm = :gdpr_sm,</v>
-      </c>
-      <c r="D74" t="str">
-        <f t="shared" si="44"/>
-        <v>"gdpr_sm" =&gt; $member-&gt;gdpr_sm,</v>
-      </c>
-      <c r="H74" t="str">
-        <f t="shared" si="45"/>
-        <v>$this-&gt;gdpr_sm = $row['gdpr_sm'];</v>
-      </c>
-      <c r="L74" t="str">
-        <f t="shared" si="46"/>
-        <v>$member-&gt;gdpr_sm = $data-&gt;gdpr_sm;</v>
+        <v>$item-&gt;gdpr_sm = $data-&gt;gdpr_sm;</v>
       </c>
       <c r="R74" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>0,</v>
       </c>
       <c r="S74">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="T74" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>,SUM(0) as sum_0</v>
       </c>
       <c r="U74" s="1" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>,AVG(0) as avg_0</v>
       </c>
     </row>

</xml_diff>